<commit_message>
EXP_V3 | 20_03_25 | 23:35
</commit_message>
<xml_diff>
--- a/03_BOM/EXP_V3_BOM.xlsx
+++ b/03_BOM/EXP_V3_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_WorkSpace\EXP_V3\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A21760-AF06-48CF-80F1-AE03FE4355FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B019A4F-11AB-4331-94E8-AE1A88C37CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="268">
   <si>
     <t>Name</t>
   </si>
@@ -377,9 +377,6 @@
     <t>jumper2</t>
   </si>
   <si>
-    <t>JP1, JP2</t>
-  </si>
-  <si>
     <t>SRP7050TA-220M</t>
   </si>
   <si>
@@ -596,24 +593,9 @@
     <t>RES SMD 16.5K OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>R108</t>
-  </si>
-  <si>
     <t>ERJ-3EKF1652V</t>
   </si>
   <si>
-    <t>19.1k 1%</t>
-  </si>
-  <si>
-    <t>RES SMD 19.1K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R109</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF1912V</t>
-  </si>
-  <si>
     <t>10k/DNP</t>
   </si>
   <si>
@@ -632,18 +614,6 @@
     <t>Texas Instruments</t>
   </si>
   <si>
-    <t>S2303</t>
-  </si>
-  <si>
-    <t>TVS DIODE 3.3VWM 8VC SOT233</t>
-  </si>
-  <si>
-    <t>TVS3, TVS4</t>
-  </si>
-  <si>
-    <t>Sangdest Microelectronics</t>
-  </si>
-  <si>
     <t>TPS259470ARPWR</t>
   </si>
   <si>
@@ -770,21 +740,9 @@
     <t>8MHz</t>
   </si>
   <si>
-    <t>Crystal, 8 MHz, -30 to 85 degC, 3.2 x 2.5 x 0.9 mm SMD</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
-    <t>XT4-16.000MHz-4_V</t>
-  </si>
-  <si>
-    <t>ECS International</t>
-  </si>
-  <si>
-    <t>ECS-80-8-33Q-ADS</t>
-  </si>
-  <si>
     <t>C1, C2, C8, C9, C12, C13, C17, C18</t>
   </si>
   <si>
@@ -827,12 +785,6 @@
     <t>R3, R9, R14, R17, R25, R26, R27, R28, R33, R34, R35, R36, R46, R62, R63, R64, R65, R70, R71, R76, R77, R82, R83, R88, R89, R98, R101, R104, R110, R135, R149</t>
   </si>
   <si>
-    <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R141, R142, R143, R144</t>
-  </si>
-  <si>
-    <t>R5, R37, R40, R90, R91, R92, R93, R99, R100, R139, R140, R145, R146, R147, R148</t>
-  </si>
-  <si>
     <t>R13, R58, R59, R60, R61</t>
   </si>
   <si>
@@ -842,9 +794,6 @@
     <t>Yageo</t>
   </si>
   <si>
-    <t>sot23-12_3</t>
-  </si>
-  <si>
     <t>VQFN-HR-10</t>
   </si>
   <si>
@@ -861,6 +810,33 @@
   </si>
   <si>
     <t>CONN HEADER SMD R/A 11POS 1.25MM</t>
+  </si>
+  <si>
+    <t>XTAL_ECS-250-12-33Q-JES-TR</t>
+  </si>
+  <si>
+    <t>ECS-250-12-33Q-JES-TR</t>
+  </si>
+  <si>
+    <t>CRYSTAL 25.0000MHZ 12PF SMD</t>
+  </si>
+  <si>
+    <t>ECS Inc.</t>
+  </si>
+  <si>
+    <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R141, R142, R143, R144</t>
+  </si>
+  <si>
+    <t>R5, R37, R40, R41, R42, R43, R44, R90, R91, R92, R93, R99, R100, R139, R140, R145, R146, R147, R148</t>
+  </si>
+  <si>
+    <t>R108, R109</t>
+  </si>
+  <si>
+    <t>JP1, JP2, JP3</t>
+  </si>
+  <si>
+    <t>Backup</t>
   </si>
 </sst>
 </file>
@@ -1162,10 +1138,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V1018"/>
+  <dimension ref="A1:V1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1152,7 @@
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1255,16 +1231,16 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="D3" s="4">
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -1392,7 +1368,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="D7" s="4">
         <v>68</v>
@@ -1530,7 +1506,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="D11" s="4">
         <v>18</v>
@@ -1639,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>57</v>
@@ -1673,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>61</v>
@@ -1707,7 +1683,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>65</v>
@@ -1741,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>65</v>
@@ -1775,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>65</v>
@@ -1809,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>65</v>
@@ -1895,7 +1871,7 @@
         <v>532611571</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>89</v>
@@ -2065,7 +2041,7 @@
         <v>86</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -2134,7 +2110,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>112</v>
@@ -2160,13 +2136,13 @@
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>114</v>
+        <v>266</v>
       </c>
       <c r="D30" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2183,25 +2159,25 @@
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>119</v>
-      </c>
       <c r="G31" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H31" s="4"/>
       <c r="M31" s="5"/>
@@ -2217,25 +2193,25 @@
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D32" s="4">
         <v>4</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H32" s="4"/>
       <c r="M32" s="5"/>
@@ -2251,25 +2227,25 @@
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="D33" s="4">
         <v>1</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H33" s="4"/>
       <c r="M33" s="5"/>
@@ -2285,25 +2261,25 @@
     </row>
     <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="F34" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="H34" s="4"/>
       <c r="J34" s="5"/>
@@ -2320,25 +2296,25 @@
     </row>
     <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="D35" s="4">
         <v>4</v>
       </c>
       <c r="E35" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>137</v>
-      </c>
       <c r="G35" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H35" s="4"/>
       <c r="M35" s="5"/>
@@ -2354,25 +2330,25 @@
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="D36" s="4">
         <v>1</v>
       </c>
       <c r="E36" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F36" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F36" s="6" t="s">
+      <c r="G36" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="H36" s="4"/>
       <c r="J36" s="5"/>
@@ -2390,25 +2366,25 @@
     </row>
     <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="4" t="s">
         <v>145</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>146</v>
       </c>
       <c r="D37" s="4">
         <v>2</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="G37" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H37" s="4"/>
       <c r="J37" s="5"/>
@@ -2426,25 +2402,25 @@
     </row>
     <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="C38" s="4" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="D38" s="4">
         <v>31</v>
       </c>
       <c r="E38" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="G38" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H38" s="4"/>
       <c r="J38" s="5"/>
@@ -2462,25 +2438,25 @@
     </row>
     <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D39" s="4">
+        <v>69</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D39" s="4">
-        <v>59</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="H39" s="4"/>
       <c r="J39" s="5"/>
@@ -2498,25 +2474,25 @@
     </row>
     <row r="40" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D40" s="4">
+        <v>19</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G40" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="D40" s="4">
-        <v>15</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="H40" s="4"/>
       <c r="J40" s="5"/>
@@ -2534,25 +2510,25 @@
     </row>
     <row r="41" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="D41" s="4">
         <v>1</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="G41" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H41" s="4"/>
       <c r="J41" s="5"/>
@@ -2570,25 +2546,25 @@
     </row>
     <row r="42" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>163</v>
       </c>
       <c r="D42" s="4">
         <v>3</v>
       </c>
       <c r="E42" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="G42" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H42" s="4"/>
       <c r="J42" s="5"/>
@@ -2605,25 +2581,25 @@
     </row>
     <row r="43" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>167</v>
       </c>
       <c r="D43" s="4">
         <v>5</v>
       </c>
       <c r="E43" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F43" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="G43" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H43" s="4"/>
       <c r="J43" s="5"/>
@@ -2640,25 +2616,25 @@
     </row>
     <row r="44" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>171</v>
       </c>
       <c r="D44" s="4">
         <v>1</v>
       </c>
       <c r="E44" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F44" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="G44" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H44" s="4"/>
       <c r="J44" s="5"/>
@@ -2676,25 +2652,25 @@
     </row>
     <row r="45" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="C45" s="4" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="D45" s="4">
         <v>5</v>
       </c>
       <c r="E45" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F45" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F45" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="G45" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H45" s="4"/>
       <c r="J45" s="5"/>
@@ -2712,25 +2688,25 @@
     </row>
     <row r="46" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>178</v>
       </c>
       <c r="D46" s="4">
         <v>1</v>
       </c>
       <c r="E46" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F46" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="G46" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H46" s="4"/>
       <c r="J46" s="5"/>
@@ -2748,25 +2724,25 @@
     </row>
     <row r="47" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F47" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F47" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="G47" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H47" s="4"/>
       <c r="J47" s="5"/>
@@ -2783,25 +2759,25 @@
     </row>
     <row r="48" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>182</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
       </c>
       <c r="E48" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>184</v>
       </c>
       <c r="H48" s="4"/>
       <c r="M48" s="5"/>
@@ -2817,25 +2793,25 @@
     </row>
     <row r="49" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D49" s="4">
+        <v>2</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="D49" s="4">
-        <v>1</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="H49" s="4"/>
       <c r="J49" s="5"/>
@@ -2852,28 +2828,27 @@
     </row>
     <row r="50" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="4">
+        <v>2</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D50" s="4">
-        <v>1</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>141</v>
-      </c>
       <c r="F50" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="G50" s="4" t="s">
         <v>192</v>
       </c>
+      <c r="G50" s="8" t="s">
+        <v>188</v>
+      </c>
       <c r="H50" s="4"/>
-      <c r="J50" s="5"/>
       <c r="K50" s="3"/>
       <c r="M50" s="5"/>
       <c r="N50" s="5"/>
@@ -2882,69 +2857,68 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
       <c r="S50" s="6"/>
-      <c r="T50" s="4"/>
+      <c r="T50" s="8"/>
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
     </row>
     <row r="51" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="D51" s="4">
         <v>2</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>194</v>
+        <v>253</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="H51" s="4"/>
-      <c r="K51" s="3"/>
+      <c r="J51" s="5"/>
       <c r="M51" s="5"/>
       <c r="N51" s="5"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
-      <c r="S51" s="6"/>
-      <c r="T51" s="8"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="4"/>
       <c r="U51" s="4"/>
       <c r="V51" s="4"/>
     </row>
     <row r="52" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D52" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>269</v>
+        <v>196</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H52" s="4"/>
-      <c r="K52" s="3"/>
       <c r="M52" s="5"/>
       <c r="N52" s="5"/>
       <c r="O52" s="4"/>
@@ -2958,28 +2932,27 @@
     </row>
     <row r="53" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D53" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>270</v>
+        <v>202</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H53" s="4"/>
-      <c r="J53" s="5"/>
       <c r="M53" s="5"/>
       <c r="N53" s="5"/>
       <c r="O53" s="4"/>
@@ -2993,27 +2966,28 @@
     </row>
     <row r="54" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D54" s="4">
+        <v>4</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F54" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D54" s="4">
-        <v>1</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>198</v>
-      </c>
       <c r="G54" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H54" s="4"/>
+      <c r="J54" s="5"/>
       <c r="M54" s="5"/>
       <c r="N54" s="5"/>
       <c r="O54" s="4"/>
@@ -3027,25 +3001,25 @@
     </row>
     <row r="55" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>209</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>211</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H55" s="4"/>
       <c r="M55" s="5"/>
@@ -3061,28 +3035,27 @@
     </row>
     <row r="56" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>214</v>
+        <v>257</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D56" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="H56" s="4"/>
-      <c r="J56" s="5"/>
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
       <c r="O56" s="4"/>
@@ -3096,27 +3069,28 @@
     </row>
     <row r="57" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D57" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H57" s="4"/>
+      <c r="J57" s="5"/>
       <c r="M57" s="5"/>
       <c r="N57" s="5"/>
       <c r="O57" s="4"/>
@@ -3130,27 +3104,28 @@
     </row>
     <row r="58" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>272</v>
+        <v>216</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>274</v>
+        <v>217</v>
       </c>
       <c r="C58" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D58" s="4">
+        <v>2</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="D58" s="4">
-        <v>1</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="G58" s="4" t="s">
-        <v>272</v>
+        <v>216</v>
       </c>
       <c r="H58" s="4"/>
+      <c r="J58" s="5"/>
       <c r="M58" s="5"/>
       <c r="N58" s="5"/>
       <c r="O58" s="4"/>
@@ -3173,19 +3148,18 @@
         <v>223</v>
       </c>
       <c r="D59" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>224</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>198</v>
+        <v>225</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="H59" s="4"/>
-      <c r="J59" s="5"/>
       <c r="M59" s="5"/>
       <c r="N59" s="5"/>
       <c r="O59" s="4"/>
@@ -3199,28 +3173,27 @@
     </row>
     <row r="60" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B60" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D60" s="4">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D60" s="4">
-        <v>2</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>229</v>
-      </c>
       <c r="F60" s="4" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="H60" s="4"/>
-      <c r="J60" s="5"/>
       <c r="M60" s="5"/>
       <c r="N60" s="5"/>
       <c r="O60" s="4"/>
@@ -3234,25 +3207,25 @@
     </row>
     <row r="61" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="C61" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>233</v>
       </c>
       <c r="D61" s="4">
         <v>1</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="G61" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="H61" s="4"/>
       <c r="M61" s="5"/>
@@ -3261,34 +3234,35 @@
       <c r="P61" s="4"/>
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
-      <c r="S61" s="4"/>
-      <c r="T61" s="4"/>
+      <c r="S61" s="6"/>
+      <c r="T61" s="6"/>
       <c r="U61" s="4"/>
       <c r="V61" s="4"/>
     </row>
     <row r="62" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D62" s="4">
         <v>1</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>198</v>
+        <v>262</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="H62" s="4"/>
+      <c r="K62" s="3"/>
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
       <c r="O62" s="4"/>
@@ -3301,28 +3275,14 @@
       <c r="V62" s="4"/>
     </row>
     <row r="63" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="D63" s="4">
-        <v>1</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="H63" s="4"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="K63" s="3"/>
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
       <c r="O63" s="4"/>
@@ -3336,28 +3296,26 @@
     </row>
     <row r="64" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>246</v>
+        <v>267</v>
       </c>
       <c r="D64" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>248</v>
+        <v>226</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="H64" s="4"/>
-      <c r="K64" s="3"/>
+        <v>255</v>
+      </c>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
       <c r="O64" s="4"/>
@@ -3390,15 +3348,20 @@
       <c r="V65" s="4"/>
     </row>
     <row r="66" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="M66" s="5"/>
-      <c r="N66" s="5"/>
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="4"/>
+      <c r="L66" s="4"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="4"/>
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
       <c r="Q66" s="4"/>
@@ -3409,22 +3372,26 @@
       <c r="V66" s="4"/>
     </row>
     <row r="67" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="K67" s="3"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="5"/>
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
       <c r="O67" s="4"/>
       <c r="P67" s="4"/>
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
-      <c r="S67" s="6"/>
-      <c r="T67" s="6"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
       <c r="U67" s="4"/>
       <c r="V67" s="4"/>
     </row>
@@ -3525,13 +3492,13 @@
       <c r="V71" s="4"/>
     </row>
     <row r="72" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7"/>
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
       <c r="C72" s="4"/>
-      <c r="D72" s="7"/>
+      <c r="D72" s="4"/>
       <c r="E72" s="4"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="7"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
@@ -3549,13 +3516,13 @@
       <c r="V72" s="4"/>
     </row>
     <row r="73" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7"/>
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="7"/>
+      <c r="D73" s="4"/>
       <c r="E73" s="4"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="7"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
@@ -26204,54 +26171,6 @@
       <c r="U1016" s="4"/>
       <c r="V1016" s="4"/>
     </row>
-    <row r="1017" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1017" s="4"/>
-      <c r="B1017" s="4"/>
-      <c r="C1017" s="4"/>
-      <c r="D1017" s="4"/>
-      <c r="E1017" s="4"/>
-      <c r="F1017" s="4"/>
-      <c r="G1017" s="4"/>
-      <c r="H1017" s="4"/>
-      <c r="I1017" s="4"/>
-      <c r="J1017" s="4"/>
-      <c r="K1017" s="4"/>
-      <c r="L1017" s="4"/>
-      <c r="M1017" s="4"/>
-      <c r="N1017" s="4"/>
-      <c r="O1017" s="4"/>
-      <c r="P1017" s="4"/>
-      <c r="Q1017" s="4"/>
-      <c r="R1017" s="4"/>
-      <c r="S1017" s="4"/>
-      <c r="T1017" s="4"/>
-      <c r="U1017" s="4"/>
-      <c r="V1017" s="4"/>
-    </row>
-    <row r="1018" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1018" s="4"/>
-      <c r="B1018" s="4"/>
-      <c r="C1018" s="4"/>
-      <c r="D1018" s="4"/>
-      <c r="E1018" s="4"/>
-      <c r="F1018" s="4"/>
-      <c r="G1018" s="4"/>
-      <c r="H1018" s="4"/>
-      <c r="I1018" s="4"/>
-      <c r="J1018" s="4"/>
-      <c r="K1018" s="4"/>
-      <c r="L1018" s="4"/>
-      <c r="M1018" s="4"/>
-      <c r="N1018" s="4"/>
-      <c r="O1018" s="4"/>
-      <c r="P1018" s="4"/>
-      <c r="Q1018" s="4"/>
-      <c r="R1018" s="4"/>
-      <c r="S1018" s="4"/>
-      <c r="T1018" s="4"/>
-      <c r="U1018" s="4"/>
-      <c r="V1018" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EXP_V3 | 25_03_25 | 14:11
</commit_message>
<xml_diff>
--- a/03_BOM/EXP_V3_BOM.xlsx
+++ b/03_BOM/EXP_V3_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_WorkSpace\EXP_V3\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B019A4F-11AB-4331-94E8-AE1A88C37CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645A4A9D-2A7D-4FD3-BBA3-EA26CB2EAB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="269">
   <si>
     <t>Name</t>
   </si>
@@ -737,9 +737,6 @@
     <t>Fujitsu</t>
   </si>
   <si>
-    <t>8MHz</t>
-  </si>
-  <si>
     <t>X1</t>
   </si>
   <si>
@@ -752,9 +749,6 @@
     <t>Kyocera AVX</t>
   </si>
   <si>
-    <t>C7, C11, C16, C19, C20, C21, C36, C37, C38, C39, C60, C61, C62, C63, C70, C75, C78, C85, C86, C87, C88, C89, C90, C91, C92, C93, C94, C95, C96, C97, C98, C99, C100, C101, C102, C103, C104, C105, C106, C107, C108, C109, C110, C111, C112, C113, C114, C115, C116, C118, C120, C126, C127, C129, C130, C136, C137, C138, C143, C144, C145, C146, C148, C149, C152, C153, C155, C156</t>
-  </si>
-  <si>
     <t>C42, C43, C44, C45, C66, C67, C68, C69, C76, C77, C79, C80, C81, C82, C117, C119, C123, C124</t>
   </si>
   <si>
@@ -773,9 +767,6 @@
     <t>ESQ-107-37-G-D</t>
   </si>
   <si>
-    <t>JUMPER</t>
-  </si>
-  <si>
     <t>L-SMD-M-3.5x3.5x2mm</t>
   </si>
   <si>
@@ -833,10 +824,22 @@
     <t>R108, R109</t>
   </si>
   <si>
-    <t>JP1, JP2, JP3</t>
-  </si>
-  <si>
     <t>Backup</t>
+  </si>
+  <si>
+    <t>C7, C11, C16, C19, C20, C21, C36, C37, C38, C39, C60, C61, C62, C63, C70, C75, C78, C85, C86, C87, C88, C89, C90, C91, C92, C93, C94, C95, C96, C97, C98, C99, C100, C101, C102, C103, C104, C105, C106, C107, C108, C109, C110, C111, C112, C113, C114, C115, C116, C118, C120, C126, C127, C129, C130, C136, C138, C143, C144, C146, C148, C149, C152, C153, C155, C156</t>
+  </si>
+  <si>
+    <t>JP1, JP2</t>
+  </si>
+  <si>
+    <t>25MHz</t>
+  </si>
+  <si>
+    <t>JUMPER _TRON</t>
+  </si>
+  <si>
+    <t>JUMPER_VUONG</t>
   </si>
 </sst>
 </file>
@@ -1138,10 +1141,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V1016"/>
+  <dimension ref="A1:V1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1231,16 +1234,16 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D3" s="4">
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>237</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>238</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -1367,11 +1370,11 @@
       <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="D7" s="4">
-        <v>68</v>
+      <c r="C7" t="s">
+        <v>264</v>
+      </c>
+      <c r="D7">
+        <v>66</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>18</v>
@@ -1506,7 +1509,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D11" s="4">
         <v>18</v>
@@ -1615,7 +1618,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>57</v>
@@ -1649,7 +1652,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>61</v>
@@ -1683,7 +1686,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>65</v>
@@ -1717,7 +1720,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>65</v>
@@ -1751,7 +1754,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>65</v>
@@ -1785,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>65</v>
@@ -1823,6 +1826,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
@@ -1871,7 +1875,7 @@
         <v>532611571</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>89</v>
@@ -2024,6 +2028,7 @@
       </c>
       <c r="H26" s="4"/>
       <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
@@ -2041,7 +2046,7 @@
         <v>86</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -2087,6 +2092,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
@@ -2110,7 +2116,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>112</v>
@@ -2136,18 +2142,19 @@
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D30" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
@@ -2158,27 +2165,21 @@
       <c r="V30" s="4"/>
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>115</v>
-      </c>
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>114</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
@@ -2186,32 +2187,32 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D32" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F32" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="4" t="s">
-        <v>122</v>
+      <c r="G32" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="H32" s="4"/>
       <c r="M32" s="5"/>
@@ -2220,32 +2221,32 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D33" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>126</v>
+        <v>244</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>118</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H33" s="4"/>
       <c r="M33" s="5"/>
@@ -2261,25 +2262,25 @@
     </row>
     <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>248</v>
+        <v>126</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H34" s="4"/>
       <c r="J34" s="5"/>
@@ -2296,25 +2297,25 @@
     </row>
     <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D35" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>136</v>
+        <v>245</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H35" s="4"/>
       <c r="M35" s="5"/>
@@ -2323,32 +2324,32 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
-      <c r="S35" s="6"/>
+      <c r="S35" s="4"/>
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D36" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>132</v>
       </c>
       <c r="H36" s="4"/>
       <c r="J36" s="5"/>
@@ -2360,22 +2361,22 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
       <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
+      <c r="T36" s="4"/>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
     </row>
     <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D37" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>140</v>
@@ -2383,8 +2384,8 @@
       <c r="F37" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>146</v>
+      <c r="G37" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="H37" s="4"/>
       <c r="J37" s="5"/>
@@ -2396,22 +2397,22 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
       <c r="S37" s="6"/>
-      <c r="T37" s="4"/>
+      <c r="T37" s="6"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
     </row>
     <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>249</v>
+        <v>145</v>
       </c>
       <c r="D38" s="4">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>140</v>
@@ -2419,8 +2420,8 @@
       <c r="F38" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>149</v>
+      <c r="G38" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="H38" s="4"/>
       <c r="J38" s="5"/>
@@ -2432,22 +2433,22 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
       <c r="S38" s="6"/>
-      <c r="T38" s="6"/>
+      <c r="T38" s="4"/>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
     </row>
     <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="D39" s="4">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>140</v>
@@ -2456,7 +2457,7 @@
         <v>141</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H39" s="4"/>
       <c r="J39" s="5"/>
@@ -2472,18 +2473,18 @@
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
     </row>
-    <row r="40" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D40" s="4">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>140</v>
@@ -2492,7 +2493,7 @@
         <v>141</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H40" s="4"/>
       <c r="J40" s="5"/>
@@ -2510,25 +2511,25 @@
     </row>
     <row r="41" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>158</v>
+        <v>261</v>
       </c>
       <c r="D41" s="4">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G41" s="4" t="s">
-        <v>159</v>
+      <c r="G41" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="H41" s="4"/>
       <c r="J41" s="5"/>
@@ -2539,23 +2540,23 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="4"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
     </row>
     <row r="42" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D42" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>140</v>
@@ -2564,7 +2565,7 @@
         <v>141</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H42" s="4"/>
       <c r="J42" s="5"/>
@@ -2581,25 +2582,25 @@
     </row>
     <row r="43" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D43" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F43" s="4" t="s">
         <v>141</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H43" s="4"/>
       <c r="J43" s="5"/>
@@ -2609,23 +2610,23 @@
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
-      <c r="S43" s="6"/>
+      <c r="S43" s="4"/>
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
     </row>
     <row r="44" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D44" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>140</v>
@@ -2633,8 +2634,8 @@
       <c r="F44" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>171</v>
+      <c r="G44" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="H44" s="4"/>
       <c r="J44" s="5"/>
@@ -2646,22 +2647,22 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
       <c r="S44" s="6"/>
-      <c r="T44" s="6"/>
+      <c r="T44" s="4"/>
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
     </row>
     <row r="45" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>250</v>
+        <v>170</v>
       </c>
       <c r="D45" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>140</v>
@@ -2670,7 +2671,7 @@
         <v>141</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H45" s="4"/>
       <c r="J45" s="5"/>
@@ -2688,16 +2689,16 @@
     </row>
     <row r="46" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>177</v>
+        <v>247</v>
       </c>
       <c r="D46" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>140</v>
@@ -2705,8 +2706,8 @@
       <c r="F46" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G46" s="4" t="s">
-        <v>178</v>
+      <c r="G46" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="H46" s="4"/>
       <c r="J46" s="5"/>
@@ -2718,19 +2719,19 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
       <c r="S46" s="6"/>
-      <c r="T46" s="4"/>
+      <c r="T46" s="6"/>
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
     </row>
     <row r="47" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>187</v>
+      <c r="A47" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>251</v>
+        <v>177</v>
       </c>
       <c r="D47" s="4">
         <v>1</v>
@@ -2738,46 +2739,47 @@
       <c r="E47" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F47" s="4" t="s">
+      <c r="F47" s="6" t="s">
         <v>141</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="H47" s="4"/>
       <c r="J47" s="5"/>
       <c r="K47" s="3"/>
       <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
       <c r="O47" s="4"/>
       <c r="P47" s="4"/>
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
+      <c r="S47" s="6"/>
       <c r="T47" s="4"/>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
     </row>
     <row r="48" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="5" t="s">
-        <v>179</v>
+      <c r="A48" t="s">
+        <v>187</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>181</v>
+        <v>248</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>182</v>
+        <v>140</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>252</v>
+        <v>141</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="H48" s="4"/>
       <c r="M48" s="5"/>
@@ -2793,25 +2795,25 @@
     </row>
     <row r="49" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>265</v>
+        <v>181</v>
       </c>
       <c r="D49" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>186</v>
+        <v>182</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="H49" s="4"/>
       <c r="J49" s="5"/>
@@ -2821,32 +2823,32 @@
       <c r="P49" s="4"/>
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
-      <c r="S49" s="6"/>
-      <c r="T49" s="6"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="4"/>
       <c r="U49" s="4"/>
       <c r="V49" s="4"/>
     </row>
     <row r="50" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>190</v>
+        <v>262</v>
       </c>
       <c r="D50" s="4">
         <v>2</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>191</v>
+        <v>140</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>188</v>
+        <v>141</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="H50" s="4"/>
       <c r="K50" s="3"/>
@@ -2857,31 +2859,31 @@
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
       <c r="S50" s="6"/>
-      <c r="T50" s="8"/>
+      <c r="T50" s="6"/>
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
     </row>
     <row r="51" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D51" s="4">
         <v>2</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F51" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="G51" s="4" t="s">
-        <v>193</v>
+      <c r="G51" s="8" t="s">
+        <v>188</v>
       </c>
       <c r="H51" s="4"/>
       <c r="J51" s="5"/>
@@ -2891,32 +2893,32 @@
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
-      <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
+      <c r="S51" s="6"/>
+      <c r="T51" s="8"/>
       <c r="U51" s="4"/>
       <c r="V51" s="4"/>
     </row>
     <row r="52" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D52" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>196</v>
+        <v>250</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>192</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="H52" s="4"/>
       <c r="M52" s="5"/>
@@ -2932,25 +2934,25 @@
     </row>
     <row r="53" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D53" s="4">
         <v>1</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>192</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H53" s="4"/>
       <c r="M53" s="5"/>
@@ -2966,25 +2968,25 @@
     </row>
     <row r="54" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D54" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H54" s="4"/>
       <c r="J54" s="5"/>
@@ -3001,25 +3003,25 @@
     </row>
     <row r="55" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D55" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>206</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="H55" s="4"/>
       <c r="M55" s="5"/>
@@ -3035,25 +3037,25 @@
     </row>
     <row r="56" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56" s="4">
         <v>1</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>255</v>
+        <v>207</v>
       </c>
       <c r="H56" s="4"/>
       <c r="M56" s="5"/>
@@ -3069,25 +3071,25 @@
     </row>
     <row r="57" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>212</v>
+        <v>254</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D57" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>215</v>
+        <v>252</v>
       </c>
       <c r="H57" s="4"/>
       <c r="J57" s="5"/>
@@ -3104,25 +3106,25 @@
     </row>
     <row r="58" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D58" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H58" s="4"/>
       <c r="J58" s="5"/>
@@ -3139,25 +3141,25 @@
     </row>
     <row r="59" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D59" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H59" s="4"/>
       <c r="M59" s="5"/>
@@ -3173,25 +3175,25 @@
     </row>
     <row r="60" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D60" s="4">
         <v>1</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>192</v>
+        <v>225</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="H60" s="4"/>
       <c r="M60" s="5"/>
@@ -3207,25 +3209,25 @@
     </row>
     <row r="61" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D61" s="4">
         <v>1</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>230</v>
+        <v>227</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>227</v>
       </c>
       <c r="H61" s="4"/>
       <c r="M61" s="5"/>
@@ -3234,32 +3236,32 @@
       <c r="P61" s="4"/>
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
-      <c r="S61" s="6"/>
-      <c r="T61" s="6"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
       <c r="U61" s="4"/>
       <c r="V61" s="4"/>
     </row>
     <row r="62" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>261</v>
+        <v>231</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D62" s="4">
         <v>1</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="G62" s="4" t="s">
-        <v>260</v>
+        <v>230</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="H62" s="4"/>
       <c r="K62" s="3"/>
@@ -3269,19 +3271,34 @@
       <c r="P62" s="4"/>
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
-      <c r="S62" s="4"/>
-      <c r="T62" s="4"/>
+      <c r="S62" s="6"/>
+      <c r="T62" s="6"/>
       <c r="U62" s="4"/>
       <c r="V62" s="4"/>
     </row>
     <row r="63" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A63" s="5"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
+      <c r="A63" t="s">
+        <v>266</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D63" s="4">
+        <v>1</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="H63" s="4"/>
       <c r="K63" s="3"/>
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
@@ -3289,85 +3306,78 @@
       <c r="P63" s="4"/>
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
-      <c r="S63" s="6"/>
-      <c r="T63" s="6"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
       <c r="U63" s="4"/>
       <c r="V63" s="4"/>
     </row>
     <row r="64" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="D64" s="4">
-        <v>2</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
       <c r="O64" s="4"/>
       <c r="P64" s="4"/>
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
-      <c r="S64" s="4"/>
-      <c r="T64" s="4"/>
+      <c r="S64" s="6"/>
+      <c r="T64" s="6"/>
       <c r="U64" s="4"/>
       <c r="V64" s="4"/>
     </row>
     <row r="65" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="K65" s="3"/>
+      <c r="A65" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D65" s="4">
+        <v>2</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>252</v>
+      </c>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
-      <c r="S65" s="6"/>
-      <c r="T65" s="6"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
       <c r="U65" s="4"/>
       <c r="V65" s="4"/>
     </row>
     <row r="66" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="7"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="K66" s="3"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
-      <c r="S66" s="4"/>
-      <c r="T66" s="4"/>
+      <c r="S66" s="6"/>
+      <c r="T66" s="6"/>
       <c r="U66" s="4"/>
       <c r="V66" s="4"/>
     </row>
@@ -3492,13 +3502,13 @@
       <c r="V71" s="4"/>
     </row>
     <row r="72" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A72" s="4"/>
-      <c r="B72" s="4"/>
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
       <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
+      <c r="D72" s="7"/>
       <c r="E72" s="4"/>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="7"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
       <c r="J72" s="4"/>
@@ -26171,6 +26181,30 @@
       <c r="U1016" s="4"/>
       <c r="V1016" s="4"/>
     </row>
+    <row r="1017" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1017" s="4"/>
+      <c r="B1017" s="4"/>
+      <c r="C1017" s="4"/>
+      <c r="D1017" s="4"/>
+      <c r="E1017" s="4"/>
+      <c r="F1017" s="4"/>
+      <c r="G1017" s="4"/>
+      <c r="H1017" s="4"/>
+      <c r="I1017" s="4"/>
+      <c r="J1017" s="4"/>
+      <c r="K1017" s="4"/>
+      <c r="L1017" s="4"/>
+      <c r="M1017" s="4"/>
+      <c r="N1017" s="4"/>
+      <c r="O1017" s="4"/>
+      <c r="P1017" s="4"/>
+      <c r="Q1017" s="4"/>
+      <c r="R1017" s="4"/>
+      <c r="S1017" s="4"/>
+      <c r="T1017" s="4"/>
+      <c r="U1017" s="4"/>
+      <c r="V1017" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EXP_V3 | 26_03_25 | 12:54
</commit_message>
<xml_diff>
--- a/03_BOM/EXP_V3_BOM.xlsx
+++ b/03_BOM/EXP_V3_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_WorkSpace\EXP_V3\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645A4A9D-2A7D-4FD3-BBA3-EA26CB2EAB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676AC6CC-4BF0-46BD-A88C-05A0E813C4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -818,9 +818,6 @@
     <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R141, R142, R143, R144</t>
   </si>
   <si>
-    <t>R5, R37, R40, R41, R42, R43, R44, R90, R91, R92, R93, R99, R100, R139, R140, R145, R146, R147, R148</t>
-  </si>
-  <si>
     <t>R108, R109</t>
   </si>
   <si>
@@ -840,6 +837,9 @@
   </si>
   <si>
     <t>JUMPER_VUONG</t>
+  </si>
+  <si>
+    <t>R5, R37, R40, R41, R42, R43, R44, R56, R90, R91, R92, R93, R99, R100, R139, R140, R145, R146, R147, R148</t>
   </si>
 </sst>
 </file>
@@ -1143,8 +1143,8 @@
   </sheetPr>
   <dimension ref="A1:V1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1371,7 @@
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D7">
         <v>66</v>
@@ -2142,13 +2142,13 @@
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D30" s="4">
         <v>2</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -2517,10 +2517,10 @@
         <v>154</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="D41" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>140</v>
@@ -2836,7 +2836,7 @@
         <v>185</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D50" s="4">
         <v>2</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="63" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>258</v>
@@ -3336,7 +3336,7 @@
         <v>254</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D65" s="4">
         <v>2</v>

</xml_diff>

<commit_message>
EXP_V120 | 09_04_25 | 20:58
</commit_message>
<xml_diff>
--- a/03_BOM/EXP_V3_BOM.xlsx
+++ b/03_BOM/EXP_V3_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_WorkSpace\EXP_V3\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676AC6CC-4BF0-46BD-A88C-05A0E813C4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551E158E-B48F-4024-ACAD-A6C7405860DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="272">
   <si>
     <t>Name</t>
   </si>
@@ -146,9 +146,6 @@
     <t>CAP CER 0.1UF 25V X7R 0603</t>
   </si>
   <si>
-    <t>C24, C25, C28, C29, C40, C41, C48, C49, C52, C53, C64, C65, C84, C122, C139, C154</t>
-  </si>
-  <si>
     <t>CL10B104KA8NNNC</t>
   </si>
   <si>
@@ -521,9 +518,6 @@
     <t>RES SMD 1K OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>R7, R19, R103</t>
-  </si>
-  <si>
     <t>ERJ-3EKF1001V</t>
   </si>
   <si>
@@ -743,9 +737,6 @@
     <t>C1, C2, C8, C9, C12, C13, C17, C18</t>
   </si>
   <si>
-    <t>TANTALUM_SMD_1206</t>
-  </si>
-  <si>
     <t>Kyocera AVX</t>
   </si>
   <si>
@@ -764,9 +755,6 @@
     <t>J10</t>
   </si>
   <si>
-    <t>ESQ-107-37-G-D</t>
-  </si>
-  <si>
     <t>L-SMD-M-3.5x3.5x2mm</t>
   </si>
   <si>
@@ -776,9 +764,6 @@
     <t>R3, R9, R14, R17, R25, R26, R27, R28, R33, R34, R35, R36, R46, R62, R63, R64, R65, R70, R71, R76, R77, R82, R83, R88, R89, R98, R101, R104, R110, R135, R149</t>
   </si>
   <si>
-    <t>R13, R58, R59, R60, R61</t>
-  </si>
-  <si>
     <t>R38</t>
   </si>
   <si>
@@ -812,12 +797,6 @@
     <t>CRYSTAL 25.0000MHZ 12PF SMD</t>
   </si>
   <si>
-    <t>ECS Inc.</t>
-  </si>
-  <si>
-    <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R141, R142, R143, R144</t>
-  </si>
-  <si>
     <t>R108, R109</t>
   </si>
   <si>
@@ -833,13 +812,43 @@
     <t>25MHz</t>
   </si>
   <si>
-    <t>JUMPER _TRON</t>
-  </si>
-  <si>
-    <t>JUMPER_VUONG</t>
-  </si>
-  <si>
     <t>R5, R37, R40, R41, R42, R43, R44, R56, R90, R91, R92, R93, R99, R100, R139, R140, R145, R146, R147, R148</t>
+  </si>
+  <si>
+    <t>TANTALUM-SMD-1206</t>
+  </si>
+  <si>
+    <t>C24, C25, C28, C29, C40, C41, C48, C49, C52, C53, C64, C65, C71, C84, C122, C139, C154</t>
+  </si>
+  <si>
+    <t>JUMPER</t>
+  </si>
+  <si>
+    <t>JUMPER2</t>
+  </si>
+  <si>
+    <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R57, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R118, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R136, R138, R141, R142, R143, R144</t>
+  </si>
+  <si>
+    <t>R7, R19, R103, R119, R150</t>
+  </si>
+  <si>
+    <t>R13, R58, R59, R60, R61, R137</t>
+  </si>
+  <si>
+    <t>TPS5430DDAR_V3</t>
+  </si>
+  <si>
+    <t>ADM3065EARZ-R7</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>SOIC8_3.9mm</t>
+  </si>
+  <si>
+    <t>ECS International</t>
   </si>
 </sst>
 </file>
@@ -1141,20 +1150,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V1017"/>
+  <dimension ref="A1:V1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.77734375" customWidth="1"/>
     <col min="2" max="2" width="62.21875" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
     <col min="7" max="7" width="26.6640625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
@@ -1192,32 +1201,28 @@
       <c r="V1" s="4"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="4"/>
-      <c r="K2" s="3"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -1227,31 +1232,28 @@
       <c r="V2" s="4"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D3">
         <v>8</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>237</v>
+      <c r="E3" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -1261,32 +1263,28 @@
       <c r="V3" s="4"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="4"/>
-      <c r="K4" s="3"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -1296,31 +1294,28 @@
       <c r="V4" s="4"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -1330,31 +1325,28 @@
       <c r="V5" s="4"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -1364,31 +1356,28 @@
       <c r="V6" s="4"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D7">
         <v>66</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H7" s="4"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -1398,31 +1387,28 @@
       <c r="V7" s="4"/>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8">
         <v>11</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>33</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1432,32 +1418,28 @@
       <c r="V8" s="4"/>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="4">
-        <v>16</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="H9" s="4"/>
-      <c r="K9" s="3"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1467,32 +1449,28 @@
       <c r="V9" s="4"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="4">
-        <v>12</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="H10" s="4"/>
-      <c r="K10" s="3"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -1502,31 +1480,28 @@
       <c r="V10" s="4"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="D11" s="4">
-        <v>18</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="H11" s="4"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -1536,32 +1511,28 @@
       <c r="V11" s="4"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="H12" s="4"/>
-      <c r="K12" s="3"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -1571,31 +1542,28 @@
       <c r="V12" s="4"/>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="4">
-        <v>2</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="H13" s="4"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -1605,31 +1573,28 @@
       <c r="V13" s="4"/>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4">
-        <v>4</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="G14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -1639,31 +1604,28 @@
       <c r="V14" s="4"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="G15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H15" s="4"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
@@ -1673,31 +1635,28 @@
       <c r="V15" s="4"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F16" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="4">
-        <v>3</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="H16" s="4"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -1707,31 +1666,28 @@
       <c r="V16" s="4"/>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="4">
-        <v>1</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="H17" s="4"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -1741,31 +1697,28 @@
       <c r="V17" s="4"/>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>74</v>
-      </c>
       <c r="H18" s="4"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -1775,31 +1728,28 @@
       <c r="V18" s="4"/>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" t="s">
         <v>76</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="H19" s="4"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
@@ -1810,24 +1760,21 @@
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="4">
-        <v>4</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="4"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -1837,31 +1784,28 @@
       <c r="V20" s="4"/>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" t="s">
         <v>83</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="G21" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H21" s="4"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
@@ -1871,31 +1815,28 @@
       <c r="V21" s="4"/>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
+      <c r="A22">
         <v>532611571</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C22" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5">
+        <v>532611571</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
-      <c r="E22" s="4">
-        <v>532611571</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>90</v>
-      </c>
       <c r="H22" s="4"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
@@ -1905,32 +1846,28 @@
       <c r="V22" s="4"/>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="A23">
         <v>532610971</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="5">
+        <v>532610971</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4">
-        <v>532610971</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="H23" s="4"/>
-      <c r="K23" s="3"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
@@ -1940,31 +1877,28 @@
       <c r="V23" s="4"/>
     </row>
     <row r="24" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="D24">
         <v>2</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>94</v>
+      <c r="E24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="H24" s="4"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
@@ -1974,28 +1908,24 @@
       <c r="V24" s="4"/>
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="4">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="K25" s="3"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -2006,30 +1936,27 @@
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="4">
-        <v>2</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>105</v>
-      </c>
       <c r="H26" s="4"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
@@ -2039,31 +1966,28 @@
       <c r="V26" s="4"/>
     </row>
     <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
+      <c r="A27">
         <v>532610271</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>239</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>532610271</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="D27" s="4">
-        <v>1</v>
-      </c>
-      <c r="E27" s="4">
-        <v>532610271</v>
-      </c>
-      <c r="F27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="G27" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="H27" s="4"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
@@ -2074,26 +1998,23 @@
     </row>
     <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" t="s">
         <v>106</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="5"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
@@ -2103,31 +2024,28 @@
       <c r="V28" s="4"/>
     </row>
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="4">
-        <v>1</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="G29" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H29" s="4"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
@@ -2138,24 +2056,21 @@
     </row>
     <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="4"/>
-      <c r="C30" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="D30" s="4">
+      <c r="C30" t="s">
+        <v>257</v>
+      </c>
+      <c r="D30">
         <v>2</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="F30" s="4"/>
+      <c r="E30" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="F30" s="5"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
@@ -2166,24 +2081,21 @@
     </row>
     <row r="31" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D31" s="4">
+      <c r="C31" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="F31" s="4"/>
+      <c r="E31" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F31" s="5"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
@@ -2193,31 +2105,28 @@
       <c r="V31" s="4"/>
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+      <c r="A32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" t="s">
         <v>115</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="4">
-        <v>1</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F32" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>114</v>
+      <c r="G32" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="H32" s="4"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -2227,31 +2136,28 @@
       <c r="V32" s="4"/>
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33">
+        <v>4</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G33" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="4">
-        <v>4</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>122</v>
-      </c>
       <c r="H33" s="4"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
@@ -2261,32 +2167,28 @@
       <c r="V33" s="4"/>
     </row>
     <row r="34" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="A34" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="C34" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>118</v>
+      <c r="F34" s="5" t="s">
+        <v>117</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H34" s="4"/>
-      <c r="J34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
@@ -2296,31 +2198,28 @@
       <c r="V34" s="4"/>
     </row>
     <row r="35" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+      <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F35" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D35" s="4">
-        <v>1</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="F35" s="4" t="s">
+      <c r="G35" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>131</v>
-      </c>
       <c r="H35" s="4"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
@@ -2330,33 +2229,28 @@
       <c r="V35" s="4"/>
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D36">
+        <v>4</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="D36" s="4">
-        <v>4</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="F36" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="G36" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H36" s="4"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="3"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
@@ -2366,33 +2260,28 @@
       <c r="V36" s="4"/>
     </row>
     <row r="37" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5" t="s">
+      <c r="A37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D37" s="4">
-        <v>1</v>
-      </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="F37" s="6" t="s">
+      <c r="G37" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="H37" s="4"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="3"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
@@ -2402,33 +2291,28 @@
       <c r="V37" s="4"/>
     </row>
     <row r="38" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
+      <c r="A38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D38" s="4">
-        <v>2</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>146</v>
-      </c>
       <c r="H38" s="4"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="3"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
@@ -2438,33 +2322,28 @@
       <c r="V38" s="4"/>
     </row>
     <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="5" t="s">
+      <c r="A39" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D39">
+        <v>31</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G39" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="D39" s="4">
-        <v>31</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="H39" s="4"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="3"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
@@ -2474,33 +2353,28 @@
       <c r="V39" s="4"/>
     </row>
     <row r="40" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="A40" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D40">
+        <v>73</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="D40" s="4">
-        <v>69</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>152</v>
-      </c>
       <c r="H40" s="4"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="3"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
@@ -2510,33 +2384,28 @@
       <c r="V40" s="4"/>
     </row>
     <row r="41" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+      <c r="A41" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="C41" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D41">
+        <v>20</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D41" s="4">
-        <v>20</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>155</v>
-      </c>
       <c r="H41" s="4"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="3"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
@@ -2546,32 +2415,28 @@
       <c r="V41" s="4"/>
     </row>
     <row r="42" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+      <c r="A42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" t="s">
         <v>157</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G42" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D42" s="4">
-        <v>1</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="H42" s="4"/>
-      <c r="J42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
@@ -2581,32 +2446,28 @@
       <c r="V42" s="4"/>
     </row>
     <row r="43" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+      <c r="A43" t="s">
+        <v>159</v>
+      </c>
+      <c r="B43" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="C43" t="s">
+        <v>265</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="D43" s="4">
-        <v>3</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="H43" s="4"/>
-      <c r="J43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -2616,33 +2477,28 @@
       <c r="V43" s="4"/>
     </row>
     <row r="44" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+      <c r="A44" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G44" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D44" s="4">
-        <v>5</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>167</v>
-      </c>
       <c r="H44" s="4"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="3"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
@@ -2652,33 +2508,28 @@
       <c r="V44" s="4"/>
     </row>
     <row r="45" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+      <c r="A45" t="s">
+        <v>166</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D45" s="4">
-        <v>1</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>171</v>
-      </c>
       <c r="H45" s="4"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="3"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="4"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
@@ -2688,33 +2539,28 @@
       <c r="V45" s="4"/>
     </row>
     <row r="46" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="A46" t="s">
+        <v>170</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D46" s="4">
-        <v>5</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>174</v>
-      </c>
       <c r="H46" s="4"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="3"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="4"/>
       <c r="P46" s="4"/>
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
@@ -2724,33 +2570,28 @@
       <c r="V46" s="4"/>
     </row>
     <row r="47" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+      <c r="A47" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C47" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D47" s="4">
-        <v>1</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>178</v>
-      </c>
       <c r="H47" s="4"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="3"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="4"/>
       <c r="P47" s="4"/>
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
@@ -2761,30 +2602,27 @@
     </row>
     <row r="48" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" t="s">
+        <v>243</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D48" s="4">
-        <v>1</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G48" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="H48" s="4"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="4"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
@@ -2794,32 +2632,28 @@
       <c r="V48" s="4"/>
     </row>
     <row r="49" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+      <c r="A49" t="s">
+        <v>177</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C49" t="s">
         <v>179</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="F49" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="G49" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D49" s="4">
-        <v>1</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="H49" s="4"/>
-      <c r="J49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="4"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
@@ -2829,32 +2663,28 @@
       <c r="V49" s="4"/>
     </row>
     <row r="50" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+      <c r="A50" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G50" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="D50" s="4">
-        <v>2</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>186</v>
-      </c>
       <c r="H50" s="4"/>
-      <c r="K50" s="3"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="4"/>
       <c r="P50" s="4"/>
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
@@ -2864,32 +2694,28 @@
       <c r="V50" s="4"/>
     </row>
     <row r="51" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+      <c r="A51" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" t="s">
         <v>188</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="F51" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="D51" s="4">
-        <v>2</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>188</v>
+      <c r="G51" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="H51" s="4"/>
-      <c r="J51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="4"/>
       <c r="P51" s="4"/>
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
@@ -2899,31 +2725,28 @@
       <c r="V51" s="4"/>
     </row>
     <row r="52" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+      <c r="A52" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C52" t="s">
         <v>193</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="D52" s="4">
+      <c r="D52">
         <v>2</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>192</v>
+      <c r="E52" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H52" s="4"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="4"/>
       <c r="P52" s="4"/>
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
@@ -2933,31 +2756,28 @@
       <c r="V52" s="4"/>
     </row>
     <row r="53" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
+      <c r="A53" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C53" t="s">
         <v>196</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D53" s="4">
+      <c r="D53">
         <v>1</v>
       </c>
-      <c r="E53" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>192</v>
+      <c r="E53" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H53" s="4"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="4"/>
       <c r="P53" s="4"/>
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
@@ -2967,32 +2787,28 @@
       <c r="V53" s="4"/>
     </row>
     <row r="54" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+      <c r="A54" t="s">
+        <v>197</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C54" t="s">
         <v>199</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C54" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D54" s="4">
-        <v>1</v>
-      </c>
-      <c r="E54" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>192</v>
+      <c r="F54" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H54" s="4"/>
-      <c r="J54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="4"/>
       <c r="P54" s="4"/>
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
@@ -3002,31 +2818,28 @@
       <c r="V54" s="4"/>
     </row>
     <row r="55" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+      <c r="A55" t="s">
+        <v>201</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C55" t="s">
         <v>203</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F55" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D55" s="4">
-        <v>4</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>206</v>
-      </c>
       <c r="G55" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H55" s="4"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="4"/>
       <c r="P55" s="4"/>
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
@@ -3036,31 +2849,28 @@
       <c r="V55" s="4"/>
     </row>
     <row r="56" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
+      <c r="A56" t="s">
+        <v>205</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C56" t="s">
         <v>207</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D56" s="4">
+      <c r="D56">
         <v>1</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>206</v>
+      <c r="E56" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>204</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H56" s="4"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="4"/>
       <c r="P56" s="4"/>
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
@@ -3070,32 +2880,25 @@
       <c r="V56" s="4"/>
     </row>
     <row r="57" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D57" s="4">
+      <c r="A57" t="s">
+        <v>268</v>
+      </c>
+      <c r="C57" t="s">
+        <v>269</v>
+      </c>
+      <c r="D57">
         <v>1</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>226</v>
+      <c r="E57" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>204</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="H57" s="4"/>
-      <c r="J57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="4"/>
       <c r="P57" s="4"/>
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
@@ -3105,32 +2908,28 @@
       <c r="V57" s="4"/>
     </row>
     <row r="58" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
-        <v>211</v>
+      <c r="A58" t="s">
+        <v>247</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D58" s="4">
-        <v>4</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="F58" s="4" t="s">
-        <v>192</v>
+        <v>249</v>
+      </c>
+      <c r="C58" t="s">
+        <v>208</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>215</v>
+        <v>247</v>
       </c>
       <c r="H58" s="4"/>
-      <c r="J58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="4"/>
       <c r="P58" s="4"/>
       <c r="Q58" s="4"/>
       <c r="R58" s="4"/>
@@ -3140,31 +2939,28 @@
       <c r="V58" s="4"/>
     </row>
     <row r="59" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
-        <v>216</v>
+      <c r="A59" t="s">
+        <v>209</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D59" s="4">
-        <v>2</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="F59" s="4" t="s">
-        <v>220</v>
+        <v>210</v>
+      </c>
+      <c r="C59" t="s">
+        <v>211</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>190</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H59" s="4"/>
-      <c r="M59" s="5"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="4"/>
       <c r="P59" s="4"/>
       <c r="Q59" s="4"/>
       <c r="R59" s="4"/>
@@ -3174,31 +2970,28 @@
       <c r="V59" s="4"/>
     </row>
     <row r="60" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
-        <v>221</v>
+      <c r="A60" t="s">
+        <v>214</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="D60" s="4">
-        <v>1</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>225</v>
+        <v>215</v>
+      </c>
+      <c r="C60" t="s">
+        <v>216</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="H60" s="4"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="4"/>
       <c r="P60" s="4"/>
       <c r="Q60" s="4"/>
       <c r="R60" s="4"/>
@@ -3208,31 +3001,28 @@
       <c r="V60" s="4"/>
     </row>
     <row r="61" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
-        <v>227</v>
+      <c r="A61" t="s">
+        <v>219</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="D61" s="4">
+        <v>220</v>
+      </c>
+      <c r="C61" t="s">
+        <v>221</v>
+      </c>
+      <c r="D61">
         <v>1</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F61" s="4" t="s">
-        <v>192</v>
+      <c r="E61" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="H61" s="4"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="4"/>
       <c r="P61" s="4"/>
       <c r="Q61" s="4"/>
       <c r="R61" s="4"/>
@@ -3242,32 +3032,28 @@
       <c r="V61" s="4"/>
     </row>
     <row r="62" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>230</v>
+      <c r="A62" t="s">
+        <v>225</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D62" s="4">
+        <v>226</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D62">
         <v>1</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="G62" s="6" t="s">
-        <v>230</v>
+      <c r="E62" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="H62" s="4"/>
-      <c r="K62" s="3"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="4"/>
       <c r="P62" s="4"/>
       <c r="Q62" s="4"/>
       <c r="R62" s="4"/>
@@ -3278,31 +3064,27 @@
     </row>
     <row r="63" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D63" s="4">
+        <v>229</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D63">
         <v>1</v>
       </c>
-      <c r="E63" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>259</v>
+      <c r="E63" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="H63" s="4"/>
-      <c r="K63" s="3"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="4"/>
       <c r="P63" s="4"/>
       <c r="Q63" s="4"/>
       <c r="R63" s="4"/>
@@ -3312,14 +3094,27 @@
       <c r="V63" s="4"/>
     </row>
     <row r="64" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="O64" s="4"/>
+      <c r="A64" t="s">
+        <v>258</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C64" t="s">
+        <v>232</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>251</v>
+      </c>
+      <c r="F64" t="s">
+        <v>271</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>252</v>
+      </c>
       <c r="P64" s="4"/>
       <c r="Q64" s="4"/>
       <c r="R64" s="4"/>
@@ -3329,79 +3124,71 @@
       <c r="V64" s="4"/>
     </row>
     <row r="65" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="D65" s="4">
-        <v>2</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F65" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
       <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
+      <c r="S65" s="6"/>
+      <c r="T65" s="6"/>
       <c r="U65" s="4"/>
       <c r="V65" s="4"/>
     </row>
     <row r="66" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="5"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="K66" s="3"/>
+      <c r="A66" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D66" s="4">
+        <v>2</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>247</v>
+      </c>
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
       <c r="Q66" s="4"/>
       <c r="R66" s="4"/>
-      <c r="S66" s="6"/>
-      <c r="T66" s="6"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="4"/>
       <c r="U66" s="4"/>
       <c r="V66" s="4"/>
     </row>
     <row r="67" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="K67" s="3"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
       <c r="O67" s="4"/>
       <c r="P67" s="4"/>
       <c r="Q67" s="4"/>
       <c r="R67" s="4"/>
-      <c r="S67" s="4"/>
-      <c r="T67" s="4"/>
+      <c r="S67" s="6"/>
+      <c r="T67" s="6"/>
       <c r="U67" s="4"/>
       <c r="V67" s="4"/>
     </row>
@@ -3526,13 +3313,13 @@
       <c r="V72" s="4"/>
     </row>
     <row r="73" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
       <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
+      <c r="D73" s="7"/>
       <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="7"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
@@ -26205,6 +25992,30 @@
       <c r="U1017" s="4"/>
       <c r="V1017" s="4"/>
     </row>
+    <row r="1018" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1018" s="4"/>
+      <c r="B1018" s="4"/>
+      <c r="C1018" s="4"/>
+      <c r="D1018" s="4"/>
+      <c r="E1018" s="4"/>
+      <c r="F1018" s="4"/>
+      <c r="G1018" s="4"/>
+      <c r="H1018" s="4"/>
+      <c r="I1018" s="4"/>
+      <c r="J1018" s="4"/>
+      <c r="K1018" s="4"/>
+      <c r="L1018" s="4"/>
+      <c r="M1018" s="4"/>
+      <c r="N1018" s="4"/>
+      <c r="O1018" s="4"/>
+      <c r="P1018" s="4"/>
+      <c r="Q1018" s="4"/>
+      <c r="R1018" s="4"/>
+      <c r="S1018" s="4"/>
+      <c r="T1018" s="4"/>
+      <c r="U1018" s="4"/>
+      <c r="V1018" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
EXP_V120 | 10_04_25 | 22:09
</commit_message>
<xml_diff>
--- a/03_BOM/EXP_V3_BOM.xlsx
+++ b/03_BOM/EXP_V3_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_WorkSpace\EXP_V3\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551E158E-B48F-4024-ACAD-A6C7405860DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F31B689-8024-4291-B838-0AA516FBA763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="273">
   <si>
     <t>Name</t>
   </si>
@@ -839,9 +839,6 @@
     <t>TPS5430DDAR_V3</t>
   </si>
   <si>
-    <t>ADM3065EARZ-R7</t>
-  </si>
-  <si>
     <t>U10</t>
   </si>
   <si>
@@ -849,6 +846,12 @@
   </si>
   <si>
     <t>ECS International</t>
+  </si>
+  <si>
+    <t>MAX3485EESA+</t>
+  </si>
+  <si>
+    <t>3.3V Powered, Â±15kV ESD-Protected, 12Mbps, Slew-Rate-Limited True RS-485/RS-422 Transceivers</t>
   </si>
 </sst>
 </file>
@@ -1152,8 +1155,8 @@
   </sheetPr>
   <dimension ref="A1:V1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J57" sqref="J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2881,22 +2884,25 @@
     </row>
     <row r="57" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>271</v>
+      </c>
+      <c r="B57" t="s">
+        <v>272</v>
+      </c>
+      <c r="C57" t="s">
         <v>268</v>
-      </c>
-      <c r="C57" t="s">
-        <v>269</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>204</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="H57" s="4"/>
       <c r="P57" s="4"/>
@@ -3110,7 +3116,7 @@
         <v>251</v>
       </c>
       <c r="F64" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>252</v>

</xml_diff>

<commit_message>
EXP_V120 | 10_04_25 | 22:24
</commit_message>
<xml_diff>
--- a/03_BOM/EXP_V3_BOM.xlsx
+++ b/03_BOM/EXP_V3_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_WorkSpace\EXP_V3\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F31B689-8024-4291-B838-0AA516FBA763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96852B63-49E1-471B-8B86-AC651579B35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -827,9 +827,6 @@
     <t>JUMPER2</t>
   </si>
   <si>
-    <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R57, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R118, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R136, R138, R141, R142, R143, R144</t>
-  </si>
-  <si>
     <t>R7, R19, R103, R119, R150</t>
   </si>
   <si>
@@ -852,6 +849,9 @@
   </si>
   <si>
     <t>3.3V Powered, Â±15kV ESD-Protected, 12Mbps, Slew-Rate-Limited True RS-485/RS-422 Transceivers</t>
+  </si>
+  <si>
+    <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R57, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R118, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R136, R138, R141, R142, R143, R144, R151</t>
   </si>
 </sst>
 </file>
@@ -1155,8 +1155,8 @@
   </sheetPr>
   <dimension ref="A1:V1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2363,10 +2363,10 @@
         <v>150</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="D40">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>139</v>
@@ -2456,7 +2456,7 @@
         <v>160</v>
       </c>
       <c r="C43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2549,7 +2549,7 @@
         <v>171</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D46">
         <v>6</v>
@@ -2772,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>190</v>
@@ -2884,25 +2884,25 @@
     </row>
     <row r="57" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>270</v>
+      </c>
+      <c r="B57" t="s">
         <v>271</v>
       </c>
-      <c r="B57" t="s">
-        <v>272</v>
-      </c>
       <c r="C57" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>204</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H57" s="4"/>
       <c r="P57" s="4"/>
@@ -3116,7 +3116,7 @@
         <v>251</v>
       </c>
       <c r="F64" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>252</v>

</xml_diff>

<commit_message>
EXP_V120 | 11_04_25 | 14:00
</commit_message>
<xml_diff>
--- a/03_BOM/EXP_V3_BOM.xlsx
+++ b/03_BOM/EXP_V3_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_WorkSpace\EXP_V3\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96852B63-49E1-471B-8B86-AC651579B35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B437378F-2C0D-483A-AA7E-15588954F6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -812,9 +812,6 @@
     <t>25MHz</t>
   </si>
   <si>
-    <t>R5, R37, R40, R41, R42, R43, R44, R56, R90, R91, R92, R93, R99, R100, R139, R140, R145, R146, R147, R148</t>
-  </si>
-  <si>
     <t>TANTALUM-SMD-1206</t>
   </si>
   <si>
@@ -852,6 +849,9 @@
   </si>
   <si>
     <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R57, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R118, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R136, R138, R141, R142, R143, R144, R151</t>
+  </si>
+  <si>
+    <t>R5, R37, R40, R41, R42, R43, R44, R56, R90, R91, R92, R93, R99, R100, R139, R140, R145, R146, R147, R148, R152</t>
   </si>
 </sst>
 </file>
@@ -1155,8 +1155,8 @@
   </sheetPr>
   <dimension ref="A1:V1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1248,7 +1248,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>234</v>
@@ -1428,7 +1428,7 @@
         <v>36</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D9">
         <v>17</v>
@@ -2069,7 +2069,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="4"/>
@@ -2094,7 +2094,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="4"/>
@@ -2363,7 +2363,7 @@
         <v>150</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D40">
         <v>74</v>
@@ -2394,10 +2394,10 @@
         <v>153</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>259</v>
+        <v>272</v>
       </c>
       <c r="D41">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>139</v>
@@ -2456,7 +2456,7 @@
         <v>160</v>
       </c>
       <c r="C43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D43">
         <v>5</v>
@@ -2549,7 +2549,7 @@
         <v>171</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D46">
         <v>6</v>
@@ -2772,7 +2772,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>190</v>
@@ -2884,25 +2884,25 @@
     </row>
     <row r="57" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>269</v>
+      </c>
+      <c r="B57" t="s">
         <v>270</v>
       </c>
-      <c r="B57" t="s">
-        <v>271</v>
-      </c>
       <c r="C57" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>204</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H57" s="4"/>
       <c r="P57" s="4"/>
@@ -3116,7 +3116,7 @@
         <v>251</v>
       </c>
       <c r="F64" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>252</v>

</xml_diff>

<commit_message>
EXP_V120 | 14_04_25 | 9:15
</commit_message>
<xml_diff>
--- a/03_BOM/EXP_V3_BOM.xlsx
+++ b/03_BOM/EXP_V3_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Altium_WorkSpace\EXP_V3\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B437378F-2C0D-483A-AA7E-15588954F6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA922ABD-819F-4EE4-B118-E0D787BAF600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="275">
   <si>
     <t>Name</t>
   </si>
@@ -848,10 +848,16 @@
     <t>3.3V Powered, Â±15kV ESD-Protected, 12Mbps, Slew-Rate-Limited True RS-485/RS-422 Transceivers</t>
   </si>
   <si>
-    <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R57, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R118, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R136, R138, R141, R142, R143, R144, R151</t>
-  </si>
-  <si>
     <t>R5, R37, R40, R41, R42, R43, R44, R56, R90, R91, R92, R93, R99, R100, R139, R140, R145, R146, R147, R148, R152</t>
+  </si>
+  <si>
+    <t>R4, R8, R15, R21, R22, R23, R24, R29, R30, R31, R32, R39, R45, R47, R48, R49, R50, R51, R52, R53, R54, R55, R66, R67, R68, R69, R72, R73, R74, R75, R78, R79, R80, R81, R84, R85, R86, R87, R94, R95, R96, R97, R105, R106, R107, R113, R114, R115, R116, R117, R120, R121, R122, R123, R124, R125, R126, R127, R128, R129, R130, R131, R132, R133, R134, R136, R138, R141, R142, R143, R144, R151</t>
+  </si>
+  <si>
+    <t>22R/DNP</t>
+  </si>
+  <si>
+    <t>R57, R118</t>
   </si>
 </sst>
 </file>
@@ -1155,8 +1161,8 @@
   </sheetPr>
   <dimension ref="A1:V1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2362,11 +2368,11 @@
       <c r="B40" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>271</v>
+      <c r="C40" t="s">
+        <v>272</v>
       </c>
       <c r="D40">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>139</v>
@@ -2394,7 +2400,7 @@
         <v>153</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D41">
         <v>21</v>
@@ -2636,25 +2642,25 @@
     </row>
     <row r="49" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>177</v>
+        <v>273</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="C49" t="s">
-        <v>179</v>
+        <v>274</v>
       </c>
       <c r="D49">
-        <v>1</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>180</v>
+        <v>2</v>
+      </c>
+      <c r="E49" t="s">
+        <v>139</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>244</v>
+        <v>140</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="H49" s="4"/>
       <c r="P49" s="4"/>
@@ -2667,25 +2673,25 @@
     </row>
     <row r="50" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>254</v>
+        <v>178</v>
+      </c>
+      <c r="C50" t="s">
+        <v>179</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>140</v>
+        <v>244</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H50" s="4"/>
       <c r="P50" s="4"/>
@@ -2698,25 +2704,25 @@
     </row>
     <row r="51" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C51" t="s">
-        <v>188</v>
+        <v>183</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="D51">
         <v>2</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H51" s="4"/>
       <c r="P51" s="4"/>
@@ -2729,25 +2735,25 @@
     </row>
     <row r="52" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C52" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D52">
         <v>2</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>245</v>
+        <v>189</v>
       </c>
       <c r="F52" s="5" t="s">
         <v>190</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H52" s="4"/>
       <c r="P52" s="4"/>
@@ -2760,25 +2766,25 @@
     </row>
     <row r="53" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C53" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>190</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H53" s="4"/>
       <c r="P53" s="4"/>
@@ -2791,25 +2797,25 @@
     </row>
     <row r="54" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C54" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>200</v>
+        <v>265</v>
       </c>
       <c r="F54" s="5" t="s">
         <v>190</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="H54" s="4"/>
       <c r="P54" s="4"/>
@@ -2822,25 +2828,25 @@
     </row>
     <row r="55" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C55" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D55">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="H55" s="4"/>
       <c r="P55" s="4"/>
@@ -2853,25 +2859,25 @@
     </row>
     <row r="56" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>205</v>
+        <v>246</v>
       </c>
       <c r="F56" s="5" t="s">
         <v>204</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H56" s="4"/>
       <c r="P56" s="4"/>
@@ -2884,25 +2890,25 @@
     </row>
     <row r="57" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>269</v>
-      </c>
-      <c r="B57" t="s">
-        <v>270</v>
+        <v>205</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>206</v>
       </c>
       <c r="C57" t="s">
-        <v>266</v>
+        <v>207</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>267</v>
+        <v>205</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>204</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>269</v>
+        <v>205</v>
       </c>
       <c r="H57" s="4"/>
       <c r="P57" s="4"/>
@@ -2915,25 +2921,25 @@
     </row>
     <row r="58" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>247</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>249</v>
+        <v>269</v>
+      </c>
+      <c r="B58" t="s">
+        <v>270</v>
       </c>
       <c r="C58" t="s">
-        <v>208</v>
+        <v>266</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>248</v>
+        <v>267</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="H58" s="4"/>
       <c r="P58" s="4"/>
@@ -2946,25 +2952,25 @@
     </row>
     <row r="59" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="C59" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D59">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>212</v>
+        <v>248</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="H59" s="4"/>
       <c r="P59" s="4"/>
@@ -2977,25 +2983,25 @@
     </row>
     <row r="60" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C60" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H60" s="4"/>
       <c r="P60" s="4"/>
@@ -3008,25 +3014,25 @@
     </row>
     <row r="61" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C61" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H61" s="4"/>
       <c r="P61" s="4"/>
@@ -3039,25 +3045,25 @@
     </row>
     <row r="62" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>227</v>
+        <v>220</v>
+      </c>
+      <c r="C62" t="s">
+        <v>221</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>190</v>
+        <v>223</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="H62" s="4"/>
       <c r="P62" s="4"/>
@@ -3070,25 +3076,25 @@
     </row>
     <row r="63" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H63" s="4"/>
       <c r="P63" s="4"/>
@@ -3101,25 +3107,25 @@
     </row>
     <row r="64" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>258</v>
+        <v>228</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C64" t="s">
-        <v>232</v>
+        <v>229</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
-      <c r="E64" t="s">
-        <v>251</v>
-      </c>
-      <c r="F64" t="s">
-        <v>268</v>
+      <c r="E64" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="P64" s="4"/>
       <c r="Q64" s="4"/>
@@ -3130,12 +3136,27 @@
       <c r="V64" s="4"/>
     </row>
     <row r="65" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
+      <c r="A65" t="s">
+        <v>258</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C65" t="s">
+        <v>232</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>251</v>
+      </c>
+      <c r="F65" t="s">
+        <v>268</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>252</v>
+      </c>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
@@ -3146,27 +3167,12 @@
       <c r="V65" s="4"/>
     </row>
     <row r="66" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="D66" s="4">
-        <v>2</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>247</v>
-      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
       <c r="M66" s="5"/>
       <c r="N66" s="5"/>
       <c r="O66" s="4"/>
@@ -3179,13 +3185,27 @@
       <c r="V66" s="4"/>
     </row>
     <row r="67" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="5"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
+      <c r="A67" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D67" s="4">
+        <v>2</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>247</v>
+      </c>
       <c r="K67" s="3"/>
       <c r="M67" s="5"/>
       <c r="N67" s="5"/>

</xml_diff>